<commit_message>
updated code to reflect changes in xlsx files.
</commit_message>
<xml_diff>
--- a/import/Diagnosis.xlsx
+++ b/import/Diagnosis.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Madhu\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Madhu\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="110">
   <si>
     <t>d.description</t>
   </si>
@@ -245,18 +245,6 @@
     <t>DIA_fc446540-7bd5-4aa4-9ded-b30b4aeb77c3</t>
   </si>
   <si>
-    <t>Warm Transfer Override</t>
-  </si>
-  <si>
-    <t>DIA_c85bca4f-9d74-40a9-bf2d-f8302d6cb16f</t>
-  </si>
-  <si>
-    <t>Warm Transfer</t>
-  </si>
-  <si>
-    <t>DIA_1ee5decd-59c7-4be1-bb2a-2854988cd348</t>
-  </si>
-  <si>
     <t>PHTFailDiag</t>
   </si>
   <si>
@@ -360,6 +348,12 @@
   </si>
   <si>
     <t>DIA_54abde23-6f53-40a3-9416-377146e50ee9</t>
+  </si>
+  <si>
+    <t>ECO Bill not Enabled</t>
+  </si>
+  <si>
+    <t>DIA_0acd4979-bc76-4f25-9d08-5315fc6bcceb</t>
   </si>
 </sst>
 </file>
@@ -451,8 +445,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -761,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection sqref="A1:E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,10 +819,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -814,10 +836,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -831,10 +853,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -848,10 +870,10 @@
         <v>0</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -865,10 +887,10 @@
         <v>0</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -882,10 +904,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -899,13 +921,13 @@
         <v>0</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="102" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -916,10 +938,10 @@
         <v>0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -933,10 +955,10 @@
         <v>0</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -950,10 +972,10 @@
         <v>0</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -967,15 +989,15 @@
         <v>0</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>5</v>
+      <c r="A13" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
@@ -984,13 +1006,13 @@
         <v>0</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="102" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -1001,10 +1023,10 @@
         <v>0</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1018,10 +1040,10 @@
         <v>0</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1035,10 +1057,10 @@
         <v>0</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1052,10 +1074,10 @@
         <v>0</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1069,10 +1091,10 @@
         <v>0</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1086,15 +1108,15 @@
         <v>0</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>40</v>
+        <v>108</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>42</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="102" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
@@ -1103,10 +1125,10 @@
         <v>0</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1120,10 +1142,10 @@
         <v>0</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1137,13 +1159,13 @@
         <v>0</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>5</v>
       </c>
@@ -1154,10 +1176,10 @@
         <v>0</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1171,10 +1193,10 @@
         <v>0</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1188,10 +1210,10 @@
         <v>0</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1205,10 +1227,10 @@
         <v>0</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1222,10 +1244,10 @@
         <v>0</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1239,13 +1261,13 @@
         <v>0</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="102" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>5</v>
       </c>
@@ -1256,10 +1278,10 @@
         <v>0</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1273,10 +1295,10 @@
         <v>0</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1290,13 +1312,13 @@
         <v>0</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="102" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>5</v>
       </c>
@@ -1307,15 +1329,15 @@
         <v>0</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>5</v>
+      <c r="A33" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="B33" s="3">
         <v>1</v>
@@ -1324,10 +1346,10 @@
         <v>0</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1341,10 +1363,10 @@
         <v>0</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1358,10 +1380,10 @@
         <v>0</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1375,13 +1397,13 @@
         <v>0</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>5</v>
       </c>
@@ -1392,10 +1414,10 @@
         <v>0</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>78</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1409,10 +1431,10 @@
         <v>0</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>80</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1426,10 +1448,10 @@
         <v>0</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>82</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1443,10 +1465,10 @@
         <v>0</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1460,10 +1482,10 @@
         <v>0</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>86</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1477,10 +1499,10 @@
         <v>0</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1494,10 +1516,10 @@
         <v>0</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1511,10 +1533,10 @@
         <v>0</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1528,10 +1550,10 @@
         <v>0</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1545,13 +1567,13 @@
         <v>0</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="102" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>5</v>
       </c>
@@ -1562,10 +1584,10 @@
         <v>0</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1579,10 +1601,10 @@
         <v>0</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1596,10 +1618,10 @@
         <v>0</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1613,15 +1635,15 @@
         <v>0</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>105</v>
+      <c r="A51" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B51" s="3">
         <v>1</v>
@@ -1630,10 +1652,10 @@
         <v>0</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>106</v>
+        <v>24</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>107</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
@@ -1647,30 +1669,14 @@
         <v>0</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B53" s="3">
-        <v>1</v>
-      </c>
-      <c r="C53" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>111</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>